<commit_message>
committing changes resulting from execution of ci-schema-convert workflow
</commit_message>
<xml_diff>
--- a/model_templates/BiospecimenMetadataTemplate.xlsx
+++ b/model_templates/BiospecimenMetadataTemplate.xlsx
@@ -27820,13 +27820,13 @@
       <formula>$I1 = "flow-sorted cells"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1000">
-    <cfRule type="expression" dxfId="0" priority="5" stopIfTrue="1">
+  <conditionalFormatting sqref="J1:J1000">
+    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>$I1 = "flow-sorted cells"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1000">
-    <cfRule type="expression" dxfId="1" priority="6" stopIfTrue="1">
+  <conditionalFormatting sqref="N1:N1000">
+    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
       <formula>$I1 = "flow-sorted cells"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27835,119 +27835,119 @@
       <formula>$I1 = "flow-sorted cells"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L1000">
+    <cfRule type="expression" dxfId="1" priority="8" stopIfTrue="1">
+      <formula>$H1 = "synovial tissue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R1:R1000">
+    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
+      <formula>$H1 = "synovial tissue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V1:V1000">
+    <cfRule type="expression" dxfId="1" priority="10" stopIfTrue="1">
+      <formula>$H1 = "synovial tissue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q1:Q1000">
+    <cfRule type="expression" dxfId="0" priority="11" stopIfTrue="1">
+      <formula>$H1 = "synovial tissue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P1:P1000">
+    <cfRule type="expression" dxfId="0" priority="12" stopIfTrue="1">
+      <formula>$H1 = "synovial tissue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1:O1000">
+    <cfRule type="expression" dxfId="0" priority="13" stopIfTrue="1">
+      <formula>$H1 = "synovial tissue"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1000">
-    <cfRule type="expression" dxfId="1" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="14" stopIfTrue="1">
+      <formula>$H1 = "synovial tissue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V1:V1000">
+    <cfRule type="expression" dxfId="1" priority="15" stopIfTrue="1">
+      <formula>$H1 = "synovial fluid"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L1000">
+    <cfRule type="expression" dxfId="1" priority="16" stopIfTrue="1">
+      <formula>$H1 = "synovial fluid"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K1000">
+    <cfRule type="expression" dxfId="1" priority="17" stopIfTrue="1">
+      <formula>$H1 = "synovial fluid"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L1000">
+    <cfRule type="expression" dxfId="1" priority="18" stopIfTrue="1">
+      <formula>$H1 = "skin biopsy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U1:U1000">
+    <cfRule type="expression" dxfId="1" priority="19" stopIfTrue="1">
+      <formula>$H1 = "skin biopsy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K1000">
+    <cfRule type="expression" dxfId="1" priority="20" stopIfTrue="1">
+      <formula>$H1 = "skin biopsy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L1000">
+    <cfRule type="expression" dxfId="1" priority="21" stopIfTrue="1">
       <formula>$H1 = "suction blister cells"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1000">
-    <cfRule type="expression" dxfId="1" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="22" stopIfTrue="1">
+      <formula>$H1 = "suction blister cells"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K1000">
+    <cfRule type="expression" dxfId="1" priority="23" stopIfTrue="1">
       <formula>$H1 = "suction blister cells"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1000">
-    <cfRule type="expression" dxfId="1" priority="10" stopIfTrue="1">
-      <formula>$H1 = "suction blister cells"</formula>
+    <cfRule type="expression" dxfId="1" priority="24" stopIfTrue="1">
+      <formula>$H1 = "suction blister fluid"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V1:V1000">
-    <cfRule type="expression" dxfId="1" priority="11" stopIfTrue="1">
-      <formula>$H1 = "synovial tissue"</formula>
+  <conditionalFormatting sqref="U1:U1000">
+    <cfRule type="expression" dxfId="1" priority="25" stopIfTrue="1">
+      <formula>$H1 = "suction blister fluid"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1000">
-    <cfRule type="expression" dxfId="1" priority="12" stopIfTrue="1">
-      <formula>$H1 = "synovial tissue"</formula>
+    <cfRule type="expression" dxfId="1" priority="26" stopIfTrue="1">
+      <formula>$H1 = "suction blister fluid"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1000">
-    <cfRule type="expression" dxfId="1" priority="13" stopIfTrue="1">
-      <formula>$H1 = "synovial tissue"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R1:R1000">
-    <cfRule type="expression" dxfId="0" priority="14" stopIfTrue="1">
-      <formula>$H1 = "synovial tissue"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O1000">
-    <cfRule type="expression" dxfId="0" priority="15" stopIfTrue="1">
-      <formula>$H1 = "synovial tissue"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P1000">
-    <cfRule type="expression" dxfId="0" priority="16" stopIfTrue="1">
-      <formula>$H1 = "synovial tissue"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:Q1000">
-    <cfRule type="expression" dxfId="0" priority="17" stopIfTrue="1">
-      <formula>$H1 = "synovial tissue"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K1000">
-    <cfRule type="expression" dxfId="1" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="27" stopIfTrue="1">
       <formula>$H1 = "skin swab"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1000">
-    <cfRule type="expression" dxfId="1" priority="19" stopIfTrue="1">
-      <formula>$H1 = "skin swab"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L1000">
-    <cfRule type="expression" dxfId="1" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="28" stopIfTrue="1">
       <formula>$H1 = "skin swab"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1000">
-    <cfRule type="expression" dxfId="1" priority="21" stopIfTrue="1">
-      <formula>$H1 = "skin biopsy"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U1:U1000">
-    <cfRule type="expression" dxfId="1" priority="22" stopIfTrue="1">
-      <formula>$H1 = "skin biopsy"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L1000">
-    <cfRule type="expression" dxfId="1" priority="23" stopIfTrue="1">
-      <formula>$H1 = "skin biopsy"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V1:V1000">
-    <cfRule type="expression" dxfId="1" priority="24" stopIfTrue="1">
-      <formula>$H1 = "synovial fluid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K1000">
-    <cfRule type="expression" dxfId="1" priority="25" stopIfTrue="1">
-      <formula>$H1 = "synovial fluid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L1000">
-    <cfRule type="expression" dxfId="1" priority="26" stopIfTrue="1">
-      <formula>$H1 = "synovial fluid"</formula>
+    <cfRule type="expression" dxfId="1" priority="29" stopIfTrue="1">
+      <formula>$H1 = "skin swab"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1000">
-    <cfRule type="expression" dxfId="1" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="30" stopIfTrue="1">
       <formula>$H1 = "saliva"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K1000">
-    <cfRule type="expression" dxfId="1" priority="28" stopIfTrue="1">
-      <formula>$H1 = "suction blister fluid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U1:U1000">
-    <cfRule type="expression" dxfId="1" priority="29" stopIfTrue="1">
-      <formula>$H1 = "suction blister fluid"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L1000">
-    <cfRule type="expression" dxfId="1" priority="30" stopIfTrue="1">
-      <formula>$H1 = "suction blister fluid"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S1000">

</xml_diff>